<commit_message>
Use std::min and std::max when perform [scale], delete unnecessary type conversion
</commit_message>
<xml_diff>
--- a/1002 - 文章中单词字典序和按行号排序/描述文档/Мэн Цзянин_3530904_90002.xlsx
+++ b/1002 - 文章中单词字典序和按行号排序/描述文档/Мэн Цзянин_3530904_90002.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4F56F6-6A90-4153-AC8C-970185284B2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F730038-C58F-4E51-9A0A-9C98DA02D9D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="3" r:id="rId1"/>
     <sheet name="BinarySearchTree.hpp" sheetId="2" r:id="rId2"/>
-    <sheet name="Error" sheetId="1" r:id="rId3"/>
-    <sheet name="Change letter" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Error" sheetId="1" r:id="rId4"/>
+    <sheet name="Change letter" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Спецификация</t>
   </si>
@@ -252,12 +253,61 @@
     <t>student</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Алгоритм</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Последовательный запрос                                                                                     (неупорядоченный связанный список)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Бинарный поиск                                                                                   (упорядоченный массив)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Бинарное дерево поиска</t>
+  </si>
+  <si>
+    <t>вставлять</t>
+  </si>
+  <si>
+    <t>найти</t>
+  </si>
+  <si>
+    <t>найти успех</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Средняя ситуация</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Худшая ситуация</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lgN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.39lgN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +359,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -324,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -611,11 +668,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -733,6 +923,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12828,7 +13063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D9D24B-FCDE-4C1B-9E07-2325E20CC54D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="Q12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="Q12" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AO42" sqref="AO42"/>
     </sheetView>
   </sheetViews>
@@ -12842,6 +13077,114 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15E1B53-0837-46D2-816C-C05EC2A7D3D7}">
+  <dimension ref="D7:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="35.4" customHeight="1"/>
+  <cols>
+    <col min="1" max="2" width="14.21875" style="20"/>
+    <col min="3" max="3" width="12.88671875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="14.21875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:8" ht="35.4" customHeight="1" thickBot="1"/>
+    <row r="8" spans="4:8" ht="35.4" customHeight="1">
+      <c r="D8" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="45"/>
+    </row>
+    <row r="9" spans="4:8" ht="35.4" customHeight="1" thickBot="1">
+      <c r="D9" s="46"/>
+      <c r="E9" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" ht="35.4" customHeight="1" thickTop="1">
+      <c r="D10" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" ht="35.4" customHeight="1">
+      <c r="D11" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" ht="35.4" customHeight="1" thickBot="1">
+      <c r="D12" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D8:D9"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M8"/>
   <sheetViews>
@@ -13010,7 +13353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FA8140-9F7A-452E-B060-748157A0451D}">
   <dimension ref="D2:J10"/>
   <sheetViews>

</xml_diff>